<commit_message>
Modul 8 - 9.4 -> Last: 'TypeScript gyakorlat'
</commit_message>
<xml_diff>
--- a/Tanulas.xlsx
+++ b/Tanulas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="113">
   <si>
     <t>Óra</t>
   </si>
@@ -310,6 +310,60 @@
   </si>
   <si>
     <t>AJAX</t>
+  </si>
+  <si>
+    <t>Framework vs library</t>
+  </si>
+  <si>
+    <t>Template engine</t>
+  </si>
+  <si>
+    <t>Virtual DOM</t>
+  </si>
+  <si>
+    <t>State of JS</t>
+  </si>
+  <si>
+    <t>Vue elméleti alapok</t>
+  </si>
+  <si>
+    <t>Vue gyakorlati alapok ( CDN, CLI, struturális felépítés, adatkötés )</t>
+  </si>
+  <si>
+    <t>Adatbeolvasás és megjelenítés</t>
+  </si>
+  <si>
+    <t>Új elem létrehozása</t>
+  </si>
+  <si>
+    <t>Komponens alapú refaktorálás</t>
+  </si>
+  <si>
+    <t>Vue gyakorlati alapok ( API kezelés, lifecycle )</t>
+  </si>
+  <si>
+    <t>Tech stack</t>
+  </si>
+  <si>
+    <t>TypeScript elmélet</t>
+  </si>
+  <si>
+    <t>TypeScript gyakorlat</t>
+  </si>
+  <si>
+    <t>Angular (projekt létrehozás (node,npm))</t>
+  </si>
+  <si>
+    <t>Angular (alkalmazás futtatás (node, ng))</t>
+  </si>
+  <si>
+    <t>Angular alapvető nyelvi elemek megismerése</t>
+  </si>
+  <si>
+    <t>Kész?</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -521,7 +575,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -575,9 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -596,7 +647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -662,9 +713,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -675,6 +723,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -975,32 +1041,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="34" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="31" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1435,11 +1501,11 @@
       <c r="D22" s="3">
         <v>52</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
       <c r="H22" s="4">
         <f>(SUM(G4:G21)+(SUM(H4:H21)/60))/60</f>
         <v>3.4141666666666666</v>
@@ -1554,11 +1620,11 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="4">
         <f>(SUM(C4:C31)+(SUM(D4:D31)/60))/60</f>
         <v>4.910277777777778</v>
@@ -1586,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,19 +1670,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-      <c r="J1" s="51" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48"/>
+      <c r="J1" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="23">
+      <c r="K1" s="47"/>
+      <c r="L1" s="55">
         <f>SUM(G4:G121)</f>
         <v>22.913333333333334</v>
       </c>
@@ -1628,13 +1694,13 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="20"/>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="52"/>
-      <c r="L2" s="23">
-        <f>SUM(G4:G65)</f>
-        <v>12.566944444444445</v>
+      <c r="K2" s="56"/>
+      <c r="L2" s="57">
+        <f>SUMIF(H4:H121, "OK", E4:E121)/3600+SUMIF(H4:H121, "OK", D4:D121)/60+SUMIF(H4:H121, "OK", C4:C121)</f>
+        <v>17.418611111111112</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1659,13 +1725,16 @@
       <c r="G3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="H3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J3" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="52"/>
-      <c r="L3" s="30">
+      <c r="K3" s="59"/>
+      <c r="L3" s="60">
         <f>L2/L1</f>
-        <v>0.54845553292600135</v>
+        <v>0.76019542236446513</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1682,12 +1751,15 @@
       <c r="E4" s="11">
         <v>48</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="51">
         <f>SUM(C4:C13)+((SUM(D4:D13)+(SUM(E4:E13)/60))/60)</f>
         <v>1.5322222222222224</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1704,8 +1776,11 @@
       <c r="E5" s="14">
         <v>4</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="54"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="8" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -1721,8 +1796,11 @@
       <c r="E6" s="14">
         <v>15</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="54"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
@@ -1738,8 +1816,11 @@
       <c r="E7" s="14">
         <v>15</v>
       </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="54"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -1755,8 +1836,11 @@
       <c r="E8" s="14">
         <v>58</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="54"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -1772,8 +1856,11 @@
       <c r="E9" s="14">
         <v>17</v>
       </c>
-      <c r="F9" s="44"/>
-      <c r="G9" s="54"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
@@ -1789,8 +1876,11 @@
       <c r="E10" s="14">
         <v>58</v>
       </c>
-      <c r="F10" s="44"/>
-      <c r="G10" s="54"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
@@ -1806,8 +1896,11 @@
       <c r="E11" s="14">
         <v>49</v>
       </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="54"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -1823,8 +1916,11 @@
       <c r="E12" s="14">
         <v>1</v>
       </c>
-      <c r="F12" s="44"/>
-      <c r="G12" s="54"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
@@ -1840,8 +1936,11 @@
       <c r="E13" s="17">
         <v>31</v>
       </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="55"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -1857,12 +1956,15 @@
       <c r="E14" s="11">
         <v>15</v>
       </c>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="44">
         <f>SUM(C14:C23)+((SUM(D14:D23)+(SUM(E14:E23)/60))/60)</f>
         <v>3.2813888888888889</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1879,8 +1981,11 @@
       <c r="E15" s="14">
         <v>32</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="46"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
@@ -1896,10 +2001,13 @@
       <c r="E16" s="14">
         <v>31</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="46"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="43"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>4</v>
       </c>
@@ -1913,10 +2021,13 @@
       <c r="E17" s="14">
         <v>53</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="46"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="43"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>5</v>
       </c>
@@ -1930,10 +2041,13 @@
       <c r="E18" s="14">
         <v>21</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="46"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="43"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>6</v>
       </c>
@@ -1947,10 +2061,13 @@
       <c r="E19" s="14">
         <v>1</v>
       </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="46"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="43"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>7</v>
       </c>
@@ -1964,10 +2081,13 @@
       <c r="E20" s="14">
         <v>45</v>
       </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="46"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="43"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>8</v>
       </c>
@@ -1981,10 +2101,13 @@
       <c r="E21" s="14">
         <v>42</v>
       </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="46"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="43"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>9</v>
       </c>
@@ -2000,10 +2123,13 @@
       <c r="E22" s="14">
         <v>45</v>
       </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="46"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="43"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>10</v>
       </c>
@@ -2017,10 +2143,13 @@
       <c r="E23" s="17">
         <v>8</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="56"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="49"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>1</v>
       </c>
@@ -2034,15 +2163,18 @@
       <c r="E24" s="19">
         <v>7</v>
       </c>
-      <c r="F24" s="43" t="s">
+      <c r="F24" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G24" s="44">
         <f>SUM(C24:C36)+((SUM(D24:D36)+(SUM(E24:E36)/60))/60)</f>
         <v>2.1827777777777779</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="22">
         <v>2</v>
       </c>
@@ -2056,10 +2188,13 @@
       <c r="E25" s="14">
         <v>5</v>
       </c>
-      <c r="F25" s="44"/>
-      <c r="G25" s="46"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="43"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="22">
         <v>3</v>
       </c>
@@ -2073,10 +2208,13 @@
       <c r="E26" s="14">
         <v>49</v>
       </c>
-      <c r="F26" s="44"/>
-      <c r="G26" s="46"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="43"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="22">
         <v>4</v>
       </c>
@@ -2090,10 +2228,13 @@
       <c r="E27" s="14">
         <v>11</v>
       </c>
-      <c r="F27" s="44"/>
-      <c r="G27" s="46"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="43"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="22">
         <v>5</v>
       </c>
@@ -2107,10 +2248,13 @@
       <c r="E28" s="14">
         <v>56</v>
       </c>
-      <c r="F28" s="44"/>
-      <c r="G28" s="46"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="43"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="22">
         <v>6</v>
       </c>
@@ -2124,10 +2268,13 @@
       <c r="E29" s="14">
         <v>53</v>
       </c>
-      <c r="F29" s="44"/>
-      <c r="G29" s="46"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="43"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="22">
         <v>7</v>
       </c>
@@ -2141,10 +2288,13 @@
       <c r="E30" s="14">
         <v>5</v>
       </c>
-      <c r="F30" s="44"/>
-      <c r="G30" s="46"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="43"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
         <v>8</v>
       </c>
@@ -2158,10 +2308,13 @@
       <c r="E31" s="14">
         <v>52</v>
       </c>
-      <c r="F31" s="44"/>
-      <c r="G31" s="46"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="43"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
         <v>9</v>
       </c>
@@ -2175,10 +2328,13 @@
       <c r="E32" s="14">
         <v>7</v>
       </c>
-      <c r="F32" s="44"/>
-      <c r="G32" s="46"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="43"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
         <v>10</v>
       </c>
@@ -2192,10 +2348,13 @@
       <c r="E33" s="14">
         <v>50</v>
       </c>
-      <c r="F33" s="44"/>
-      <c r="G33" s="46"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="43"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="22">
         <v>11</v>
       </c>
@@ -2209,10 +2368,13 @@
       <c r="E34" s="14">
         <v>50</v>
       </c>
-      <c r="F34" s="44"/>
-      <c r="G34" s="46"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="43"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="22">
         <v>12</v>
       </c>
@@ -2226,10 +2388,13 @@
       <c r="E35" s="14">
         <v>58</v>
       </c>
-      <c r="F35" s="44"/>
-      <c r="G35" s="46"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="43"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>13</v>
       </c>
@@ -2243,33 +2408,39 @@
       <c r="E36" s="17">
         <v>15</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="56"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="24">
+      <c r="F36" s="49"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="23">
         <v>1</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25">
+      <c r="C37" s="24"/>
+      <c r="D37" s="24">
         <v>0</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="24">
         <v>53</v>
       </c>
-      <c r="F37" s="43" t="s">
+      <c r="F37" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="G37" s="45">
+      <c r="G37" s="44">
         <f>SUM(C37:C45)+((SUM(D37:D45)+(SUM(E37:E45)/60))/60)</f>
         <v>1.4549999999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="26">
+      <c r="H37" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="25">
         <v>2</v>
       </c>
       <c r="B38" s="14" t="s">
@@ -2282,11 +2453,14 @@
       <c r="E38" s="14">
         <v>41</v>
       </c>
-      <c r="F38" s="44"/>
-      <c r="G38" s="46"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="26">
+      <c r="F38" s="43"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="25">
         <v>3</v>
       </c>
       <c r="B39" s="14" t="s">
@@ -2299,11 +2473,14 @@
       <c r="E39" s="14">
         <v>28</v>
       </c>
-      <c r="F39" s="44"/>
-      <c r="G39" s="46"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="26">
+      <c r="F39" s="43"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="25">
         <v>4</v>
       </c>
       <c r="B40" s="14" t="s">
@@ -2316,11 +2493,14 @@
       <c r="E40" s="14">
         <v>20</v>
       </c>
-      <c r="F40" s="44"/>
-      <c r="G40" s="46"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="26">
+      <c r="F40" s="43"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="25">
         <v>5</v>
       </c>
       <c r="B41" s="14" t="s">
@@ -2333,11 +2513,14 @@
       <c r="E41" s="14">
         <v>3</v>
       </c>
-      <c r="F41" s="44"/>
-      <c r="G41" s="46"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="26">
+      <c r="F41" s="43"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="25">
         <v>6</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -2350,11 +2533,14 @@
       <c r="E42" s="14">
         <v>4</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="46"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="26">
+      <c r="F42" s="43"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="25">
         <v>7</v>
       </c>
       <c r="B43" s="14" t="s">
@@ -2367,11 +2553,14 @@
       <c r="E43" s="14">
         <v>11</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="46"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="26">
+      <c r="F43" s="43"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="25">
         <v>8</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -2384,10 +2573,13 @@
       <c r="E44" s="14">
         <v>14</v>
       </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="46"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="43"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <v>9</v>
       </c>
@@ -2401,33 +2593,39 @@
       <c r="E45" s="17">
         <v>24</v>
       </c>
-      <c r="F45" s="44"/>
-      <c r="G45" s="46"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27">
+      <c r="F45" s="43"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="26">
         <v>1</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28">
+      <c r="C46" s="27"/>
+      <c r="D46" s="27">
         <v>1</v>
       </c>
-      <c r="E46" s="28">
+      <c r="E46" s="27">
         <v>35</v>
       </c>
-      <c r="F46" s="41" t="s">
+      <c r="F46" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="G46" s="42">
+      <c r="G46" s="41">
         <f>SUM(C46:C55)+((SUM(D46:D55)+(SUM(E46:E55)/60))/60)</f>
         <v>2.2202777777777776</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="29">
+      <c r="H46" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="28">
         <v>2</v>
       </c>
       <c r="B47" s="14" t="s">
@@ -2440,11 +2638,14 @@
       <c r="E47" s="14">
         <v>34</v>
       </c>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="29">
+      <c r="F47" s="40"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="28">
         <v>3</v>
       </c>
       <c r="B48" s="14" t="s">
@@ -2457,11 +2658,14 @@
       <c r="E48" s="14">
         <v>16</v>
       </c>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42"/>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="29">
+      <c r="F48" s="40"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="28">
         <v>4</v>
       </c>
       <c r="B49" s="14" t="s">
@@ -2474,11 +2678,14 @@
       <c r="E49" s="14">
         <v>44</v>
       </c>
-      <c r="F49" s="41"/>
-      <c r="G49" s="42"/>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="29">
+      <c r="F49" s="40"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="28">
         <v>5</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -2491,11 +2698,14 @@
       <c r="E50" s="14">
         <v>47</v>
       </c>
-      <c r="F50" s="41"/>
-      <c r="G50" s="42"/>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="29">
+      <c r="F50" s="40"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="28">
         <v>6</v>
       </c>
       <c r="B51" s="14" t="s">
@@ -2508,11 +2718,14 @@
       <c r="E51" s="14">
         <v>37</v>
       </c>
-      <c r="F51" s="41"/>
-      <c r="G51" s="42"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="29">
+      <c r="F51" s="40"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="28">
         <v>7</v>
       </c>
       <c r="B52" s="14" t="s">
@@ -2525,11 +2738,14 @@
       <c r="E52" s="14">
         <v>17</v>
       </c>
-      <c r="F52" s="41"/>
-      <c r="G52" s="42"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="29">
+      <c r="F52" s="40"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="28">
         <v>8</v>
       </c>
       <c r="B53" s="14" t="s">
@@ -2542,11 +2758,14 @@
       <c r="E53" s="14">
         <v>58</v>
       </c>
-      <c r="F53" s="41"/>
-      <c r="G53" s="42"/>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="29">
+      <c r="F53" s="40"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="28">
         <v>9</v>
       </c>
       <c r="B54" s="14" t="s">
@@ -2559,10 +2778,13 @@
       <c r="E54" s="14">
         <v>28</v>
       </c>
-      <c r="F54" s="41"/>
-      <c r="G54" s="42"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="40"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <v>10</v>
       </c>
@@ -2578,33 +2800,39 @@
       <c r="E55" s="17">
         <v>57</v>
       </c>
-      <c r="F55" s="41"/>
-      <c r="G55" s="42"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="27">
+      <c r="F55" s="40"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="26">
         <v>1</v>
       </c>
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28">
+      <c r="C56" s="27"/>
+      <c r="D56" s="27">
         <v>0</v>
       </c>
-      <c r="E56" s="28">
+      <c r="E56" s="27">
         <v>44</v>
       </c>
-      <c r="F56" s="41" t="s">
+      <c r="F56" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="G56" s="42">
+      <c r="G56" s="41">
         <f>SUM(C56:C65)+((SUM(D56:D65)+(SUM(E56:E65)/60))/60)</f>
         <v>1.8952777777777778</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="29">
+      <c r="H56" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="28">
         <v>2</v>
       </c>
       <c r="B57" s="14" t="s">
@@ -2617,11 +2845,14 @@
       <c r="E57" s="14">
         <v>41</v>
       </c>
-      <c r="F57" s="41"/>
-      <c r="G57" s="42"/>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="29">
+      <c r="F57" s="40"/>
+      <c r="G57" s="41"/>
+      <c r="H57" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="28">
         <v>3</v>
       </c>
       <c r="B58" s="14" t="s">
@@ -2634,11 +2865,14 @@
       <c r="E58" s="14">
         <v>38</v>
       </c>
-      <c r="F58" s="41"/>
-      <c r="G58" s="42"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="29">
+      <c r="F58" s="40"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="28">
         <v>4</v>
       </c>
       <c r="B59" s="14" t="s">
@@ -2651,11 +2885,14 @@
       <c r="E59" s="14">
         <v>11</v>
       </c>
-      <c r="F59" s="41"/>
-      <c r="G59" s="42"/>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="29">
+      <c r="F59" s="40"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="28">
         <v>5</v>
       </c>
       <c r="B60" s="14" t="s">
@@ -2668,11 +2905,14 @@
       <c r="E60" s="14">
         <v>1</v>
       </c>
-      <c r="F60" s="41"/>
-      <c r="G60" s="42"/>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="29">
+      <c r="F60" s="40"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="28">
         <v>6</v>
       </c>
       <c r="B61" s="14" t="s">
@@ -2685,11 +2925,14 @@
       <c r="E61" s="14">
         <v>21</v>
       </c>
-      <c r="F61" s="41"/>
-      <c r="G61" s="42"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="29">
+      <c r="F61" s="40"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="28">
         <v>7</v>
       </c>
       <c r="B62" s="14" t="s">
@@ -2702,11 +2945,14 @@
       <c r="E62" s="14">
         <v>18</v>
       </c>
-      <c r="F62" s="41"/>
-      <c r="G62" s="42"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="29">
+      <c r="F62" s="40"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="28">
         <v>8</v>
       </c>
       <c r="B63" s="14" t="s">
@@ -2719,11 +2965,14 @@
       <c r="E63" s="14">
         <v>39</v>
       </c>
-      <c r="F63" s="41"/>
-      <c r="G63" s="42"/>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="29">
+      <c r="F63" s="40"/>
+      <c r="G63" s="41"/>
+      <c r="H63" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="28">
         <v>9</v>
       </c>
       <c r="B64" s="14" t="s">
@@ -2736,10 +2985,13 @@
       <c r="E64" s="14">
         <v>22</v>
       </c>
-      <c r="F64" s="41"/>
-      <c r="G64" s="42"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F64" s="40"/>
+      <c r="G64" s="41"/>
+      <c r="H64" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>10</v>
       </c>
@@ -2753,33 +3005,39 @@
       <c r="E65" s="17">
         <v>48</v>
       </c>
-      <c r="F65" s="41"/>
-      <c r="G65" s="42"/>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="27">
+      <c r="F65" s="40"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="26">
         <v>1</v>
       </c>
-      <c r="B66" s="28" t="s">
+      <c r="B66" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28">
+      <c r="C66" s="27"/>
+      <c r="D66" s="27">
         <v>0</v>
       </c>
-      <c r="E66" s="28">
+      <c r="E66" s="27">
         <v>57</v>
       </c>
-      <c r="F66" s="41" t="s">
+      <c r="F66" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G66" s="42">
+      <c r="G66" s="41">
         <f>SUM(C66:C74)+((SUM(D66:D74)+(SUM(E66:E74)/60))/60)</f>
         <v>1.1280555555555556</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="29">
+      <c r="H66" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="28">
         <v>2</v>
       </c>
       <c r="B67" s="14" t="s">
@@ -2792,11 +3050,14 @@
       <c r="E67" s="14">
         <v>44</v>
       </c>
-      <c r="F67" s="41"/>
-      <c r="G67" s="42"/>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="29">
+      <c r="F67" s="40"/>
+      <c r="G67" s="41"/>
+      <c r="H67" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="28">
         <v>3</v>
       </c>
       <c r="B68" s="14" t="s">
@@ -2809,11 +3070,14 @@
       <c r="E68" s="14">
         <v>9</v>
       </c>
-      <c r="F68" s="41"/>
-      <c r="G68" s="42"/>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="29">
+      <c r="F68" s="40"/>
+      <c r="G68" s="41"/>
+      <c r="H68" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="28">
         <v>4</v>
       </c>
       <c r="B69" s="14" t="s">
@@ -2826,11 +3090,14 @@
       <c r="E69" s="14">
         <v>59</v>
       </c>
-      <c r="F69" s="41"/>
-      <c r="G69" s="42"/>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="29">
+      <c r="F69" s="40"/>
+      <c r="G69" s="41"/>
+      <c r="H69" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="28">
         <v>5</v>
       </c>
       <c r="B70" s="14" t="s">
@@ -2843,11 +3110,14 @@
       <c r="E70" s="14">
         <v>57</v>
       </c>
-      <c r="F70" s="41"/>
-      <c r="G70" s="42"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="29">
+      <c r="F70" s="40"/>
+      <c r="G70" s="41"/>
+      <c r="H70" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="28">
         <v>6</v>
       </c>
       <c r="B71" s="14" t="s">
@@ -2860,11 +3130,14 @@
       <c r="E71" s="14">
         <v>15</v>
       </c>
-      <c r="F71" s="41"/>
-      <c r="G71" s="42"/>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="29">
+      <c r="F71" s="40"/>
+      <c r="G71" s="41"/>
+      <c r="H71" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="28">
         <v>7</v>
       </c>
       <c r="B72" s="14" t="s">
@@ -2877,11 +3150,14 @@
       <c r="E72" s="14">
         <v>14</v>
       </c>
-      <c r="F72" s="41"/>
-      <c r="G72" s="42"/>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="29">
+      <c r="F72" s="40"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="28">
         <v>8</v>
       </c>
       <c r="B73" s="14" t="s">
@@ -2894,10 +3170,13 @@
       <c r="E73" s="14">
         <v>59</v>
       </c>
-      <c r="F73" s="41"/>
-      <c r="G73" s="42"/>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F73" s="40"/>
+      <c r="G73" s="41"/>
+      <c r="H73" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
         <v>9</v>
       </c>
@@ -2911,34 +3190,44 @@
       <c r="E74" s="17">
         <v>27</v>
       </c>
-      <c r="F74" s="41"/>
-      <c r="G74" s="42"/>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="27">
+      <c r="F74" s="40"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="26">
         <v>1</v>
       </c>
-      <c r="B75" s="28"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28">
+      <c r="B75" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27">
         <v>0</v>
       </c>
-      <c r="E75" s="28">
+      <c r="E75" s="27">
         <v>44</v>
       </c>
-      <c r="F75" s="41" t="s">
+      <c r="F75" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="G75" s="42">
+      <c r="G75" s="41">
         <f>SUM(C75:C85)+((SUM(D75:D85)+(SUM(E75:E85)/60))/60)</f>
         <v>3.0550000000000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="29">
+      <c r="H75" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="28">
         <v>2</v>
       </c>
-      <c r="B76" s="14"/>
+      <c r="B76" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="C76" s="14"/>
       <c r="D76" s="14">
         <v>35</v>
@@ -2946,14 +3235,19 @@
       <c r="E76" s="14">
         <v>30</v>
       </c>
-      <c r="F76" s="41"/>
-      <c r="G76" s="42"/>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="29">
+      <c r="F76" s="40"/>
+      <c r="G76" s="41"/>
+      <c r="H76" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="28">
         <v>3</v>
       </c>
-      <c r="B77" s="14"/>
+      <c r="B77" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="C77" s="14"/>
       <c r="D77" s="14">
         <v>12</v>
@@ -2961,14 +3255,19 @@
       <c r="E77" s="14">
         <v>32</v>
       </c>
-      <c r="F77" s="41"/>
-      <c r="G77" s="42"/>
-    </row>
-    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="29">
+      <c r="F77" s="40"/>
+      <c r="G77" s="41"/>
+      <c r="H77" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="28">
         <v>4</v>
       </c>
-      <c r="B78" s="14"/>
+      <c r="B78" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="C78" s="14"/>
       <c r="D78" s="14">
         <v>5</v>
@@ -2976,14 +3275,19 @@
       <c r="E78" s="14">
         <v>49</v>
       </c>
-      <c r="F78" s="41"/>
-      <c r="G78" s="42"/>
-    </row>
-    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="29">
+      <c r="F78" s="40"/>
+      <c r="G78" s="41"/>
+      <c r="H78" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="28">
         <v>5</v>
       </c>
-      <c r="B79" s="14"/>
+      <c r="B79" s="14" t="s">
+        <v>98</v>
+      </c>
       <c r="C79" s="14"/>
       <c r="D79" s="14">
         <v>5</v>
@@ -2991,14 +3295,19 @@
       <c r="E79" s="14">
         <v>46</v>
       </c>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-    </row>
-    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="29">
+      <c r="F79" s="40"/>
+      <c r="G79" s="41"/>
+      <c r="H79" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="28">
         <v>6</v>
       </c>
-      <c r="B80" s="14"/>
+      <c r="B80" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="C80" s="14"/>
       <c r="D80" s="14">
         <v>8</v>
@@ -3006,14 +3315,19 @@
       <c r="E80" s="14">
         <v>37</v>
       </c>
-      <c r="F80" s="41"/>
-      <c r="G80" s="42"/>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="29">
+      <c r="F80" s="40"/>
+      <c r="G80" s="41"/>
+      <c r="H80" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="28">
         <v>7</v>
       </c>
-      <c r="B81" s="14"/>
+      <c r="B81" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="C81" s="14"/>
       <c r="D81" s="14">
         <v>17</v>
@@ -3021,14 +3335,19 @@
       <c r="E81" s="14">
         <v>13</v>
       </c>
-      <c r="F81" s="41"/>
-      <c r="G81" s="42"/>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="29">
+      <c r="F81" s="40"/>
+      <c r="G81" s="41"/>
+      <c r="H81" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="28">
         <v>8</v>
       </c>
-      <c r="B82" s="14"/>
+      <c r="B82" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="C82" s="14"/>
       <c r="D82" s="14">
         <v>16</v>
@@ -3036,14 +3355,19 @@
       <c r="E82" s="14">
         <v>6</v>
       </c>
-      <c r="F82" s="41"/>
-      <c r="G82" s="42"/>
-    </row>
-    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="29">
+      <c r="F82" s="40"/>
+      <c r="G82" s="41"/>
+      <c r="H82" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="28">
         <v>9</v>
       </c>
-      <c r="B83" s="14"/>
+      <c r="B83" s="14" t="s">
+        <v>101</v>
+      </c>
       <c r="C83" s="14"/>
       <c r="D83" s="14">
         <v>37</v>
@@ -3051,14 +3375,19 @@
       <c r="E83" s="14">
         <v>54</v>
       </c>
-      <c r="F83" s="41"/>
-      <c r="G83" s="42"/>
-    </row>
-    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="29">
+      <c r="F83" s="40"/>
+      <c r="G83" s="41"/>
+      <c r="H83" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="28">
         <v>10</v>
       </c>
-      <c r="B84" s="14"/>
+      <c r="B84" s="14" t="s">
+        <v>102</v>
+      </c>
       <c r="C84" s="14"/>
       <c r="D84" s="14">
         <v>23</v>
@@ -3066,14 +3395,19 @@
       <c r="E84" s="14">
         <v>34</v>
       </c>
-      <c r="F84" s="41"/>
-      <c r="G84" s="42"/>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F84" s="40"/>
+      <c r="G84" s="41"/>
+      <c r="H84" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15">
         <v>11</v>
       </c>
-      <c r="B85" s="17"/>
+      <c r="B85" s="14" t="s">
+        <v>103</v>
+      </c>
       <c r="C85" s="17"/>
       <c r="D85" s="17">
         <v>19</v>
@@ -3081,34 +3415,44 @@
       <c r="E85" s="17">
         <v>33</v>
       </c>
-      <c r="F85" s="41"/>
-      <c r="G85" s="42"/>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="27">
+      <c r="F85" s="40"/>
+      <c r="G85" s="41"/>
+      <c r="H85" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="26">
         <v>1</v>
       </c>
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28">
+      <c r="B86" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27">
         <v>0</v>
       </c>
-      <c r="E86" s="28">
+      <c r="E86" s="27">
         <v>35</v>
       </c>
-      <c r="F86" s="41" t="s">
+      <c r="F86" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="G86" s="42">
+      <c r="G86" s="41">
         <f>SUM(C86:C92)+((SUM(D86:D92)+(SUM(E86:E92)/60))/60)</f>
         <v>1.1788888888888889</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="29">
+      <c r="H86" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="28">
         <v>2</v>
       </c>
-      <c r="B87" s="14"/>
+      <c r="B87" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="C87" s="14"/>
       <c r="D87" s="14">
         <v>13</v>
@@ -3116,14 +3460,19 @@
       <c r="E87" s="14">
         <v>2</v>
       </c>
-      <c r="F87" s="41"/>
-      <c r="G87" s="42"/>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="29">
+      <c r="F87" s="40"/>
+      <c r="G87" s="41"/>
+      <c r="H87" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="28">
         <v>3</v>
       </c>
-      <c r="B88" s="14"/>
+      <c r="B88" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="C88" s="14"/>
       <c r="D88" s="14">
         <v>4</v>
@@ -3131,14 +3480,19 @@
       <c r="E88" s="14">
         <v>48</v>
       </c>
-      <c r="F88" s="41"/>
-      <c r="G88" s="42"/>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="29">
+      <c r="F88" s="40"/>
+      <c r="G88" s="41"/>
+      <c r="H88" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="28">
         <v>4</v>
       </c>
-      <c r="B89" s="14"/>
+      <c r="B89" s="14" t="s">
+        <v>107</v>
+      </c>
       <c r="C89" s="14"/>
       <c r="D89" s="14">
         <v>21</v>
@@ -3146,14 +3500,19 @@
       <c r="E89" s="14">
         <v>42</v>
       </c>
-      <c r="F89" s="41"/>
-      <c r="G89" s="42"/>
-    </row>
-    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="29">
+      <c r="F89" s="40"/>
+      <c r="G89" s="41"/>
+      <c r="H89" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="28">
         <v>5</v>
       </c>
-      <c r="B90" s="14"/>
+      <c r="B90" s="14" t="s">
+        <v>108</v>
+      </c>
       <c r="C90" s="14"/>
       <c r="D90" s="14">
         <v>9</v>
@@ -3161,14 +3520,16 @@
       <c r="E90" s="14">
         <v>15</v>
       </c>
-      <c r="F90" s="41"/>
-      <c r="G90" s="42"/>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="29">
+      <c r="F90" s="40"/>
+      <c r="G90" s="41"/>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="28">
         <v>6</v>
       </c>
-      <c r="B91" s="14"/>
+      <c r="B91" s="14" t="s">
+        <v>109</v>
+      </c>
       <c r="C91" s="14"/>
       <c r="D91" s="14">
         <v>4</v>
@@ -3176,14 +3537,16 @@
       <c r="E91" s="14">
         <v>25</v>
       </c>
-      <c r="F91" s="41"/>
-      <c r="G91" s="42"/>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F91" s="40"/>
+      <c r="G91" s="41"/>
+    </row>
+    <row r="92" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="15">
         <v>7</v>
       </c>
-      <c r="B92" s="17"/>
+      <c r="B92" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="C92" s="17"/>
       <c r="D92" s="17">
         <v>16</v>
@@ -3191,31 +3554,31 @@
       <c r="E92" s="17">
         <v>57</v>
       </c>
-      <c r="F92" s="41"/>
-      <c r="G92" s="42"/>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="27">
+      <c r="F92" s="40"/>
+      <c r="G92" s="41"/>
+    </row>
+    <row r="93" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="26">
         <v>1</v>
       </c>
-      <c r="B93" s="28"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28">
+      <c r="B93" s="27"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27">
         <v>2</v>
       </c>
-      <c r="E93" s="28">
+      <c r="E93" s="27">
         <v>39</v>
       </c>
-      <c r="F93" s="41" t="s">
+      <c r="F93" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="G93" s="42">
+      <c r="G93" s="41">
         <f>SUM(C93:C99)+((SUM(D93:D99)+(SUM(E93:E99)/60))/60)</f>
         <v>0.90722222222222226</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="29">
+    <row r="94" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="28">
         <v>2</v>
       </c>
       <c r="B94" s="14"/>
@@ -3226,11 +3589,12 @@
       <c r="E94" s="14">
         <v>13</v>
       </c>
-      <c r="F94" s="41"/>
-      <c r="G94" s="42"/>
-    </row>
-    <row r="95" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="29">
+      <c r="F94" s="40"/>
+      <c r="G94" s="41"/>
+      <c r="H94" s="29"/>
+    </row>
+    <row r="95" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="28">
         <v>3</v>
       </c>
       <c r="B95" s="14"/>
@@ -3241,11 +3605,12 @@
       <c r="E95" s="14">
         <v>25</v>
       </c>
-      <c r="F95" s="41"/>
-      <c r="G95" s="42"/>
-    </row>
-    <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="29">
+      <c r="F95" s="40"/>
+      <c r="G95" s="41"/>
+      <c r="H95" s="29"/>
+    </row>
+    <row r="96" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="28">
         <v>4</v>
       </c>
       <c r="B96" s="14"/>
@@ -3256,11 +3621,12 @@
       <c r="E96" s="14">
         <v>42</v>
       </c>
-      <c r="F96" s="41"/>
-      <c r="G96" s="42"/>
-    </row>
-    <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="29">
+      <c r="F96" s="40"/>
+      <c r="G96" s="41"/>
+      <c r="H96" s="29"/>
+    </row>
+    <row r="97" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="28">
         <v>5</v>
       </c>
       <c r="B97" s="14"/>
@@ -3271,11 +3637,12 @@
       <c r="E97" s="14">
         <v>39</v>
       </c>
-      <c r="F97" s="41"/>
-      <c r="G97" s="42"/>
-    </row>
-    <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="29">
+      <c r="F97" s="40"/>
+      <c r="G97" s="41"/>
+      <c r="H97" s="29"/>
+    </row>
+    <row r="98" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="28">
         <v>6</v>
       </c>
       <c r="B98" s="14"/>
@@ -3286,10 +3653,11 @@
       <c r="E98" s="14">
         <v>54</v>
       </c>
-      <c r="F98" s="41"/>
-      <c r="G98" s="42"/>
-    </row>
-    <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F98" s="40"/>
+      <c r="G98" s="41"/>
+      <c r="H98" s="29"/>
+    </row>
+    <row r="99" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="15">
         <v>7</v>
       </c>
@@ -3301,31 +3669,33 @@
       <c r="E99" s="17">
         <v>54</v>
       </c>
-      <c r="F99" s="41"/>
-      <c r="G99" s="42"/>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="27">
+      <c r="F99" s="40"/>
+      <c r="G99" s="41"/>
+      <c r="H99" s="29"/>
+    </row>
+    <row r="100" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="26">
         <v>1</v>
       </c>
-      <c r="B100" s="28"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28">
+      <c r="B100" s="27"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27">
         <v>5</v>
       </c>
-      <c r="E100" s="28">
+      <c r="E100" s="27">
         <v>5</v>
       </c>
-      <c r="F100" s="41" t="s">
+      <c r="F100" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="G100" s="42">
+      <c r="G100" s="41">
         <f>SUM(C100:C109)+((SUM(D100:D109)+(SUM(E100:E109)/60))/60)</f>
         <v>2.0394444444444444</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="29">
+      <c r="H100" s="29"/>
+    </row>
+    <row r="101" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="28">
         <v>2</v>
       </c>
       <c r="B101" s="14"/>
@@ -3336,11 +3706,12 @@
       <c r="E101" s="14">
         <v>24</v>
       </c>
-      <c r="F101" s="41"/>
-      <c r="G101" s="42"/>
-    </row>
-    <row r="102" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="29">
+      <c r="F101" s="40"/>
+      <c r="G101" s="41"/>
+      <c r="H101" s="29"/>
+    </row>
+    <row r="102" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="28">
         <v>3</v>
       </c>
       <c r="B102" s="14"/>
@@ -3351,11 +3722,12 @@
       <c r="E102" s="14">
         <v>52</v>
       </c>
-      <c r="F102" s="41"/>
-      <c r="G102" s="42"/>
-    </row>
-    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="29">
+      <c r="F102" s="40"/>
+      <c r="G102" s="41"/>
+      <c r="H102" s="29"/>
+    </row>
+    <row r="103" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="28">
         <v>4</v>
       </c>
       <c r="B103" s="14"/>
@@ -3366,11 +3738,12 @@
       <c r="E103" s="14">
         <v>14</v>
       </c>
-      <c r="F103" s="41"/>
-      <c r="G103" s="42"/>
-    </row>
-    <row r="104" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="29">
+      <c r="F103" s="40"/>
+      <c r="G103" s="41"/>
+      <c r="H103" s="29"/>
+    </row>
+    <row r="104" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="28">
         <v>5</v>
       </c>
       <c r="B104" s="14"/>
@@ -3381,11 +3754,12 @@
       <c r="E104" s="14">
         <v>10</v>
       </c>
-      <c r="F104" s="41"/>
-      <c r="G104" s="42"/>
-    </row>
-    <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="29">
+      <c r="F104" s="40"/>
+      <c r="G104" s="41"/>
+      <c r="H104" s="29"/>
+    </row>
+    <row r="105" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="28">
         <v>6</v>
       </c>
       <c r="B105" s="14"/>
@@ -3396,11 +3770,12 @@
       <c r="E105" s="14">
         <v>41</v>
       </c>
-      <c r="F105" s="41"/>
-      <c r="G105" s="42"/>
-    </row>
-    <row r="106" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="29">
+      <c r="F105" s="40"/>
+      <c r="G105" s="41"/>
+      <c r="H105" s="29"/>
+    </row>
+    <row r="106" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="28">
         <v>7</v>
       </c>
       <c r="B106" s="14"/>
@@ -3411,11 +3786,12 @@
       <c r="E106" s="14">
         <v>51</v>
       </c>
-      <c r="F106" s="41"/>
-      <c r="G106" s="42"/>
-    </row>
-    <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="29">
+      <c r="F106" s="40"/>
+      <c r="G106" s="41"/>
+      <c r="H106" s="29"/>
+    </row>
+    <row r="107" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="28">
         <v>8</v>
       </c>
       <c r="B107" s="14"/>
@@ -3426,11 +3802,12 @@
       <c r="E107" s="14">
         <v>14</v>
       </c>
-      <c r="F107" s="41"/>
-      <c r="G107" s="42"/>
-    </row>
-    <row r="108" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="29">
+      <c r="F107" s="40"/>
+      <c r="G107" s="41"/>
+      <c r="H107" s="29"/>
+    </row>
+    <row r="108" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="28">
         <v>9</v>
       </c>
       <c r="B108" s="14"/>
@@ -3441,10 +3818,11 @@
       <c r="E108" s="14">
         <v>24</v>
       </c>
-      <c r="F108" s="41"/>
-      <c r="G108" s="42"/>
-    </row>
-    <row r="109" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F108" s="40"/>
+      <c r="G108" s="41"/>
+      <c r="H108" s="29"/>
+    </row>
+    <row r="109" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="15">
         <v>10</v>
       </c>
@@ -3456,31 +3834,33 @@
       <c r="E109" s="17">
         <v>27</v>
       </c>
-      <c r="F109" s="41"/>
-      <c r="G109" s="42"/>
-    </row>
-    <row r="110" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="27">
+      <c r="F109" s="40"/>
+      <c r="G109" s="41"/>
+      <c r="H109" s="29"/>
+    </row>
+    <row r="110" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="26">
         <v>1</v>
       </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28">
+      <c r="B110" s="27"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27">
         <v>12</v>
       </c>
-      <c r="E110" s="28">
+      <c r="E110" s="27">
         <v>28</v>
       </c>
-      <c r="F110" s="41" t="s">
+      <c r="F110" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="G110" s="42">
+      <c r="G110" s="41">
         <f>SUM(C110:C121)+((SUM(D110:D121)+(SUM(E110:E121)/60))/60)</f>
         <v>2.0377777777777779</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="29">
+      <c r="H110" s="29"/>
+    </row>
+    <row r="111" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="28">
         <v>2</v>
       </c>
       <c r="B111" s="14"/>
@@ -3491,11 +3871,12 @@
       <c r="E111" s="14">
         <v>4</v>
       </c>
-      <c r="F111" s="41"/>
-      <c r="G111" s="42"/>
-    </row>
-    <row r="112" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="29">
+      <c r="F111" s="40"/>
+      <c r="G111" s="41"/>
+      <c r="H111" s="29"/>
+    </row>
+    <row r="112" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="28">
         <v>3</v>
       </c>
       <c r="B112" s="14"/>
@@ -3506,11 +3887,12 @@
       <c r="E112" s="14">
         <v>10</v>
       </c>
-      <c r="F112" s="41"/>
-      <c r="G112" s="42"/>
-    </row>
-    <row r="113" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="29">
+      <c r="F112" s="40"/>
+      <c r="G112" s="41"/>
+      <c r="H112" s="29"/>
+    </row>
+    <row r="113" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="28">
         <v>4</v>
       </c>
       <c r="B113" s="14"/>
@@ -3521,11 +3903,12 @@
       <c r="E113" s="14">
         <v>0</v>
       </c>
-      <c r="F113" s="41"/>
-      <c r="G113" s="42"/>
-    </row>
-    <row r="114" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="29">
+      <c r="F113" s="40"/>
+      <c r="G113" s="41"/>
+      <c r="H113" s="29"/>
+    </row>
+    <row r="114" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="28">
         <v>5</v>
       </c>
       <c r="B114" s="14"/>
@@ -3536,11 +3919,12 @@
       <c r="E114" s="14">
         <v>17</v>
       </c>
-      <c r="F114" s="41"/>
-      <c r="G114" s="42"/>
-    </row>
-    <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="29">
+      <c r="F114" s="40"/>
+      <c r="G114" s="41"/>
+      <c r="H114" s="29"/>
+    </row>
+    <row r="115" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="28">
         <v>6</v>
       </c>
       <c r="B115" s="14"/>
@@ -3551,11 +3935,12 @@
       <c r="E115" s="14">
         <v>18</v>
       </c>
-      <c r="F115" s="41"/>
-      <c r="G115" s="42"/>
-    </row>
-    <row r="116" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="29">
+      <c r="F115" s="40"/>
+      <c r="G115" s="41"/>
+      <c r="H115" s="29"/>
+    </row>
+    <row r="116" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="28">
         <v>7</v>
       </c>
       <c r="B116" s="14"/>
@@ -3566,11 +3951,12 @@
       <c r="E116" s="14">
         <v>1</v>
       </c>
-      <c r="F116" s="41"/>
-      <c r="G116" s="42"/>
-    </row>
-    <row r="117" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="29">
+      <c r="F116" s="40"/>
+      <c r="G116" s="41"/>
+      <c r="H116" s="29"/>
+    </row>
+    <row r="117" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="28">
         <v>8</v>
       </c>
       <c r="B117" s="14"/>
@@ -3581,11 +3967,12 @@
       <c r="E117" s="14">
         <v>44</v>
       </c>
-      <c r="F117" s="41"/>
-      <c r="G117" s="42"/>
-    </row>
-    <row r="118" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="29">
+      <c r="F117" s="40"/>
+      <c r="G117" s="41"/>
+      <c r="H117" s="29"/>
+    </row>
+    <row r="118" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="28">
         <v>9</v>
       </c>
       <c r="B118" s="14"/>
@@ -3596,11 +3983,12 @@
       <c r="E118" s="14">
         <v>2</v>
       </c>
-      <c r="F118" s="41"/>
-      <c r="G118" s="42"/>
-    </row>
-    <row r="119" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="29">
+      <c r="F118" s="40"/>
+      <c r="G118" s="41"/>
+      <c r="H118" s="29"/>
+    </row>
+    <row r="119" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="28">
         <v>10</v>
       </c>
       <c r="B119" s="14"/>
@@ -3611,11 +3999,12 @@
       <c r="E119" s="14">
         <v>11</v>
       </c>
-      <c r="F119" s="41"/>
-      <c r="G119" s="42"/>
-    </row>
-    <row r="120" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="29">
+      <c r="F119" s="40"/>
+      <c r="G119" s="41"/>
+      <c r="H119" s="29"/>
+    </row>
+    <row r="120" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="28">
         <v>11</v>
       </c>
       <c r="B120" s="14"/>
@@ -3626,10 +4015,11 @@
       <c r="E120" s="14">
         <v>40</v>
       </c>
-      <c r="F120" s="41"/>
-      <c r="G120" s="42"/>
-    </row>
-    <row r="121" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F120" s="40"/>
+      <c r="G120" s="41"/>
+      <c r="H120" s="29"/>
+    </row>
+    <row r="121" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="15">
         <v>12</v>
       </c>
@@ -3641,10 +4031,11 @@
       <c r="E121" s="17">
         <v>21</v>
       </c>
-      <c r="F121" s="41"/>
-      <c r="G121" s="42"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F121" s="40"/>
+      <c r="G121" s="41"/>
+      <c r="H121" s="29"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D123" s="14"/>
       <c r="E123" s="14"/>
     </row>

</xml_diff>